<commit_message>
Added GF1301-081, GF1302-081, GF1303-081, GF1304-081
</commit_message>
<xml_diff>
--- a/Doc/ReportList.xlsx
+++ b/Doc/ReportList.xlsx
@@ -132,12 +132,12 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
-  <fonts count="23">
+  <fonts count="22">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -162,6 +162,13 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF006100"/>
       <name val="宋体"/>
       <charset val="134"/>
@@ -169,9 +176,41 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
       <name val="宋体"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -191,9 +230,17 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="134"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -205,11 +252,40 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -228,89 +304,6 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="34">
     <fill>
@@ -339,54 +332,78 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -429,12 +446,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -459,19 +470,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -490,24 +501,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -616,11 +609,41 @@
       <diagonal/>
     </border>
     <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
       <bottom style="medium">
         <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -636,30 +659,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -688,21 +687,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top style="thin">
@@ -713,153 +697,162 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="17" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="21" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="11" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="15" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="15" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="20" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="20" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="11" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -891,10 +884,7 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="31" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="31" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="5" xfId="7" applyBorder="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="7" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -903,7 +893,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="7" applyBorder="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="7" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
@@ -912,7 +902,10 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="31" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="7" applyBorder="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="31" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="31" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1261,7 +1254,7 @@
   <dimension ref="A1:C29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="2"/>
@@ -1316,7 +1309,7 @@
       <c r="B5" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="9" t="s">
+      <c r="C5" s="8" t="s">
         <v>5</v>
       </c>
     </row>
@@ -1325,7 +1318,7 @@
       <c r="B6" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="9" t="s">
+      <c r="C6" s="8" t="s">
         <v>5</v>
       </c>
     </row>
@@ -1334,7 +1327,7 @@
       <c r="B7" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="10" t="s">
+      <c r="C7" s="9" t="s">
         <v>11</v>
       </c>
     </row>
@@ -1343,21 +1336,21 @@
       <c r="B8" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="C8" s="10" t="s">
+      <c r="C8" s="9" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="9" ht="14.25" spans="1:3">
-      <c r="A9" s="11"/>
-      <c r="B9" s="12" t="s">
+      <c r="A9" s="10"/>
+      <c r="B9" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="C9" s="13" t="s">
+      <c r="C9" s="12" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="10" spans="1:3">
-      <c r="A10" s="14" t="s">
+      <c r="A10" s="13" t="s">
         <v>14</v>
       </c>
       <c r="B10" s="4" t="s">
@@ -1377,16 +1370,16 @@
       </c>
     </row>
     <row r="12" ht="14.25" spans="1:3">
-      <c r="A12" s="11"/>
-      <c r="B12" s="12" t="s">
+      <c r="A12" s="10"/>
+      <c r="B12" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="C12" s="15" t="s">
+      <c r="C12" s="14" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="13" spans="1:3">
-      <c r="A13" s="14" t="s">
+      <c r="A13" s="13" t="s">
         <v>18</v>
       </c>
       <c r="B13" s="4" t="s">
@@ -1423,24 +1416,24 @@
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="1:3">
-      <c r="A17" s="11"/>
-      <c r="B17" s="12" t="s">
+    <row r="17" ht="14.25" spans="1:3">
+      <c r="A17" s="10"/>
+      <c r="B17" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="C17" s="9" t="s">
+      <c r="C17" s="14" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="18" spans="1:3">
-      <c r="A18" s="14" t="s">
+      <c r="A18" s="13" t="s">
         <v>24</v>
       </c>
       <c r="B18" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="C18" s="16" t="s">
-        <v>11</v>
+      <c r="C18" s="15" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="19" spans="1:3">
@@ -1448,7 +1441,7 @@
       <c r="B19" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="C19" s="10" t="s">
+      <c r="C19" s="9" t="s">
         <v>11</v>
       </c>
     </row>
@@ -1457,7 +1450,7 @@
       <c r="B20" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="C20" s="10" t="s">
+      <c r="C20" s="9" t="s">
         <v>11</v>
       </c>
     </row>
@@ -1466,8 +1459,8 @@
       <c r="B21" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="C21" s="10" t="s">
-        <v>11</v>
+      <c r="C21" s="16" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="22" spans="1:3">
@@ -1475,8 +1468,8 @@
       <c r="B22" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="C22" s="10" t="s">
-        <v>11</v>
+      <c r="C22" s="16" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="23" spans="1:3">
@@ -1484,8 +1477,8 @@
       <c r="B23" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="C23" s="10" t="s">
-        <v>11</v>
+      <c r="C23" s="16" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="24" spans="1:3">
@@ -1493,8 +1486,8 @@
       <c r="B24" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="C24" s="10" t="s">
-        <v>11</v>
+      <c r="C24" s="16" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="25" spans="1:3">
@@ -1502,7 +1495,7 @@
       <c r="B25" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="C25" s="10" t="s">
+      <c r="C25" s="9" t="s">
         <v>11</v>
       </c>
     </row>
@@ -1511,7 +1504,7 @@
       <c r="B26" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="C26" s="10" t="s">
+      <c r="C26" s="9" t="s">
         <v>11</v>
       </c>
     </row>
@@ -1520,7 +1513,7 @@
       <c r="B27" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="C27" s="10" t="s">
+      <c r="C27" s="9" t="s">
         <v>11</v>
       </c>
     </row>
@@ -1529,16 +1522,16 @@
       <c r="B28" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="C28" s="10" t="s">
+      <c r="C28" s="9" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="29" ht="14.25" spans="1:3">
-      <c r="A29" s="11"/>
-      <c r="B29" s="12" t="s">
+      <c r="A29" s="10"/>
+      <c r="B29" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="C29" s="13" t="s">
+      <c r="C29" s="12" t="s">
         <v>11</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updated ReportList.xlsx for GF1103-121
</commit_message>
<xml_diff>
--- a/Doc/ReportList.xlsx
+++ b/Doc/ReportList.xlsx
@@ -132,10 +132,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="22">
     <font>
@@ -177,6 +177,14 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -253,6 +261,13 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF9C6500"/>
       <name val="宋体"/>
       <charset val="134"/>
@@ -261,21 +276,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -332,6 +332,30 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -392,18 +416,30 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -429,42 +465,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -605,6 +605,21 @@
       </top>
       <bottom style="thin">
         <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -663,21 +678,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
@@ -714,10 +714,10 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="21" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="27" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -726,137 +726,137 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="12" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="14" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="11" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="15" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="15" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -900,9 +900,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="31" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="31" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="31" applyBorder="1">
@@ -1254,7 +1251,7 @@
   <dimension ref="A1:C29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E29" sqref="E29"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="2"/>
@@ -1432,7 +1429,7 @@
       <c r="B18" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="C18" s="15" t="s">
+      <c r="C18" s="5" t="s">
         <v>5</v>
       </c>
     </row>
@@ -1441,8 +1438,8 @@
       <c r="B19" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="C19" s="9" t="s">
-        <v>11</v>
+      <c r="C19" s="15" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="20" spans="1:3">
@@ -1459,7 +1456,7 @@
       <c r="B21" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="C21" s="16" t="s">
+      <c r="C21" s="8" t="s">
         <v>5</v>
       </c>
     </row>
@@ -1468,7 +1465,7 @@
       <c r="B22" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="C22" s="16" t="s">
+      <c r="C22" s="8" t="s">
         <v>5</v>
       </c>
     </row>
@@ -1477,7 +1474,7 @@
       <c r="B23" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="C23" s="16" t="s">
+      <c r="C23" s="8" t="s">
         <v>5</v>
       </c>
     </row>
@@ -1486,7 +1483,7 @@
       <c r="B24" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="C24" s="16" t="s">
+      <c r="C24" s="8" t="s">
         <v>5</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added SF6302-131 and SF6402-131
</commit_message>
<xml_diff>
--- a/Doc/ReportList.xlsx
+++ b/Doc/ReportList.xlsx
@@ -133,9 +133,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="22">
     <font>
@@ -176,9 +176,101 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF3F3F76"/>
       <name val="宋体"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -190,109 +282,17 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -338,24 +338,36 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -374,24 +386,48 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -404,13 +440,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -422,61 +470,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -605,6 +605,26 @@
       </top>
       <bottom style="thin">
         <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -639,6 +659,21 @@
       <diagonal/>
     </border>
     <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
@@ -657,15 +692,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -680,32 +706,6 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -714,10 +714,10 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -726,7 +726,7 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -735,124 +735,124 @@
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="14" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="14" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="17" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="16" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="16" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="14" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1251,7 +1251,7 @@
   <dimension ref="A1:C29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="2"/>
@@ -1501,7 +1501,7 @@
       <c r="B26" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="C26" s="15" t="s">
+      <c r="C26" s="8" t="s">
         <v>5</v>
       </c>
     </row>
@@ -1510,8 +1510,8 @@
       <c r="B27" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="C27" s="9" t="s">
-        <v>11</v>
+      <c r="C27" s="15" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="28" spans="1:3">
@@ -1519,11 +1519,11 @@
       <c r="B28" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="C28" s="9" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="29" ht="14.25" spans="1:3">
+      <c r="C28" s="15" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3">
       <c r="A29" s="10"/>
       <c r="B29" s="11" t="s">
         <v>36</v>

</xml_diff>